<commit_message>
Add final diagram for development work flow.
</commit_message>
<xml_diff>
--- a/docs/AWS_SQL_Server_Container_Hosting_Strategy_diagram - Full_Dev.xlsx
+++ b/docs/AWS_SQL_Server_Container_Hosting_Strategy_diagram - Full_Dev.xlsx
@@ -1267,6 +1267,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1569,7 +1573,7 @@
   <dimension ref="E30:E31"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+      <selection activeCell="AI9" sqref="AI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>